<commit_message>
Atualização automática de CANGUCU.xlsx
</commit_message>
<xml_diff>
--- a/CANGUCU.xlsx
+++ b/CANGUCU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{642BBB5E-E8B7-412C-B640-451D0C67E9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D731253-CF4F-4D55-BAAF-5364CEBBA5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1396,7 +1396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1457,30 +1457,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1498,7 +1474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1537,17 +1513,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1594,7 +1565,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{C1D0D184-6E40-47B3-B993-13AAB4B17807}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{B97B4AD4-CF0C-4E0A-8FD5-61E7B79A01F0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1624,10 +1595,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0351865A-5BA1-4A07-8322-9DB125E026F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{881C66A8-03EC-446A-8C48-89451A5A0A2F}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1665,7 +1636,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79E77EFB-200D-417A-BF86-09F22214C17F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5D4E902-2EFC-4AC1-9443-83F3C66D86DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1728,7 +1699,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F32AF8F-D2B8-40EE-BEFE-7703EFDE3FE5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6110747D-3BB3-4E0F-836E-139D1655ACA9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1747,7 +1718,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10657901-0E4C-1BD2-D6D4-8626CC96830F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EE73305-EECC-A6D7-F6D7-B95D789D2133}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1796,7 +1767,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A089971-C773-1551-C5CC-716EBD21C2E5}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55DCCC65-9D04-5C42-35E0-2E3D1EB563C7}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1815,7 +1786,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ADD880B-E55B-C76B-820D-2B1A2D026A49}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C81545B2-8797-490F-F91E-CFAB1D5CCA95}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1846,7 +1817,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08794511-2931-9905-C2C5-604DE48B125E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{407331EA-F0AE-3F8C-3047-68054CC44F66}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1877,7 +1848,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA301F6F-A006-6ED7-5184-5BD80759E282}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41859B09-F1BE-215D-2757-5468F39ECE0A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1920,7 +1891,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F131D7A1-D4CA-4230-B164-AB658AE3597B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0085E76-81BA-46C3-879E-D5EB63365BF9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1958,7 +1929,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3CACE16-A37F-48A1-B651-E1FA18B07973}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36F3EEFD-14EB-4CE7-8BFC-611A340515AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2001,7 +1972,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A723B38D-950D-45C5-A85F-749AA845A7F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E24D38A-303B-4745-9924-FE319A80CF2D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2314,7 +2285,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69788D7-02E0-419B-91B8-3D5A4967A1D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBA0924-0CCE-405A-95D4-669FC38088DA}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2326,98 +2297,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="41"/>
-    <col min="6" max="6" width="2" style="41" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="41" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="41"/>
+    <col min="1" max="5" width="12.5703125" style="38"/>
+    <col min="6" max="6" width="2" style="38" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="38" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="40"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="40"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="40"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="40"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="40"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="40"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="40"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="40"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="40"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="40"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="40"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="40"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="40"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="40"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="40"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="40"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="40"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="40"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="40"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="40"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="40"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="40"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="40"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="40"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="40"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="40"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="40"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="40"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="40"/>
+      <c r="F29" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5781,19 +5752,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5827,46 +5798,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>287</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>287</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>290</v>
       </c>
     </row>
@@ -5874,7 +5845,7 @@
       <c r="A2" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="19">
         <v>27604</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5886,10 +5857,10 @@
       <c r="E2" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F2" s="23">
-        <v>31</v>
-      </c>
-      <c r="G2" s="23">
+      <c r="F2" s="20">
+        <v>31</v>
+      </c>
+      <c r="G2" s="20">
         <v>310</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -5918,7 +5889,7 @@
       <c r="A3" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="19">
         <v>12708</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5930,10 +5901,10 @@
       <c r="E3" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>7.08</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>70.8</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -5962,7 +5933,7 @@
       <c r="A4" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="19">
         <v>451585</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5974,10 +5945,10 @@
       <c r="E4" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>10.35</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>103.5</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -6006,7 +5977,7 @@
       <c r="A5" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="19">
         <v>146028</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -6018,10 +5989,10 @@
       <c r="E5" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="F5" s="23">
-        <v>31</v>
-      </c>
-      <c r="G5" s="23">
+      <c r="F5" s="20">
+        <v>31</v>
+      </c>
+      <c r="G5" s="20">
         <v>310</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -6050,7 +6021,7 @@
       <c r="A6" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="19">
         <v>392814</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -6062,10 +6033,10 @@
       <c r="E6" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="20">
         <v>174.09</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>1740.92</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -6094,7 +6065,7 @@
       <c r="A7" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="19">
         <v>393204</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -6106,10 +6077,10 @@
       <c r="E7" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="20">
         <v>33.11</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>331.08</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -6138,7 +6109,7 @@
       <c r="A8" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="19">
         <v>401788</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -6150,10 +6121,10 @@
       <c r="E8" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="20">
         <v>174.09</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="20">
         <v>1740.92</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -6182,7 +6153,7 @@
       <c r="A9" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="19">
         <v>415643</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -6194,10 +6165,10 @@
       <c r="E9" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="20">
         <v>36.700000000000003</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <v>367</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -6226,7 +6197,7 @@
       <c r="A10" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="19">
         <v>416002</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -6238,10 +6209,10 @@
       <c r="E10" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <v>36.700000000000003</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="20">
         <v>367</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -6270,7 +6241,7 @@
       <c r="A11" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="19">
         <v>416023</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6282,10 +6253,10 @@
       <c r="E11" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="20">
         <v>36.700000000000003</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="20">
         <v>367</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -6314,7 +6285,7 @@
       <c r="A12" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="19">
         <v>430035</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -6326,10 +6297,10 @@
       <c r="E12" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>35.71</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="20">
         <v>357.09</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -6358,7 +6329,7 @@
       <c r="A13" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="19">
         <v>433577</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -6370,10 +6341,10 @@
       <c r="E13" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="20">
         <v>34.9</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="20">
         <v>349</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -6402,7 +6373,7 @@
       <c r="A14" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="19">
         <v>433710</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -6414,10 +6385,10 @@
       <c r="E14" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <v>34.9</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="20">
         <v>349</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -6446,7 +6417,7 @@
       <c r="A15" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="19">
         <v>433739</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -6458,10 +6429,10 @@
       <c r="E15" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="20">
         <v>34.9</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="20">
         <v>349</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -6490,7 +6461,7 @@
       <c r="A16" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="19">
         <v>433741</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -6502,10 +6473,10 @@
       <c r="E16" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="20">
         <v>34.9</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="20">
         <v>349</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -6534,7 +6505,7 @@
       <c r="A17" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="19">
         <v>418919</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -6546,10 +6517,10 @@
       <c r="E17" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="20">
         <v>53.9</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="20">
         <v>539</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -6578,7 +6549,7 @@
       <c r="A18" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="19">
         <v>418920</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -6590,10 +6561,10 @@
       <c r="E18" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="20">
         <v>53.9</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="20">
         <v>539</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -6622,7 +6593,7 @@
       <c r="A19" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="19">
         <v>418921</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -6634,10 +6605,10 @@
       <c r="E19" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="20">
         <v>319.89999999999998</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="20">
         <v>3199</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -6666,7 +6637,7 @@
       <c r="A20" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="19">
         <v>418922</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -6678,10 +6649,10 @@
       <c r="E20" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="20">
         <v>39.9</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="20">
         <v>399</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -6710,7 +6681,7 @@
       <c r="A21" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="19">
         <v>418923</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -6722,10 +6693,10 @@
       <c r="E21" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="20">
         <v>39.9</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="20">
         <v>399</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -6754,7 +6725,7 @@
       <c r="A22" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="19">
         <v>418924</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -6766,10 +6737,10 @@
       <c r="E22" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="20">
         <v>39.9</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="20">
         <v>399</v>
       </c>
       <c r="H22" s="2" t="s">
@@ -6798,7 +6769,7 @@
       <c r="A23" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="19">
         <v>418925</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -6810,10 +6781,10 @@
       <c r="E23" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="20">
         <v>39.9</v>
       </c>
-      <c r="G23" s="23">
+      <c r="G23" s="20">
         <v>399</v>
       </c>
       <c r="H23" s="2" t="s">
@@ -6842,7 +6813,7 @@
       <c r="A24" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="19">
         <v>418926</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -6854,10 +6825,10 @@
       <c r="E24" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="20">
         <v>39.9</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="20">
         <v>399</v>
       </c>
       <c r="H24" s="2" t="s">
@@ -6886,7 +6857,7 @@
       <c r="A25" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="19">
         <v>418927</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -6898,10 +6869,10 @@
       <c r="E25" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="20">
         <v>39.9</v>
       </c>
-      <c r="G25" s="23">
+      <c r="G25" s="20">
         <v>399</v>
       </c>
       <c r="H25" s="2" t="s">
@@ -6930,7 +6901,7 @@
       <c r="A26" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="19">
         <v>418928</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -6942,10 +6913,10 @@
       <c r="E26" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="20">
         <v>39.9</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26" s="20">
         <v>399</v>
       </c>
       <c r="H26" s="2" t="s">
@@ -6974,7 +6945,7 @@
       <c r="A27" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="19">
         <v>418929</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -6986,10 +6957,10 @@
       <c r="E27" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="20">
         <v>39.9</v>
       </c>
-      <c r="G27" s="23">
+      <c r="G27" s="20">
         <v>399</v>
       </c>
       <c r="H27" s="2" t="s">
@@ -7018,7 +6989,7 @@
       <c r="A28" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B28" s="19">
         <v>418930</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -7030,10 +7001,10 @@
       <c r="E28" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="20">
         <v>39.9</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="20">
         <v>399</v>
       </c>
       <c r="H28" s="2" t="s">
@@ -7062,7 +7033,7 @@
       <c r="A29" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B29" s="22">
+      <c r="B29" s="19">
         <v>418931</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -7074,10 +7045,10 @@
       <c r="E29" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="20">
         <v>39.9</v>
       </c>
-      <c r="G29" s="23">
+      <c r="G29" s="20">
         <v>399</v>
       </c>
       <c r="H29" s="2" t="s">
@@ -7106,7 +7077,7 @@
       <c r="A30" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B30" s="22">
+      <c r="B30" s="19">
         <v>418932</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -7118,10 +7089,10 @@
       <c r="E30" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="20">
         <v>39.9</v>
       </c>
-      <c r="G30" s="23">
+      <c r="G30" s="20">
         <v>399</v>
       </c>
       <c r="H30" s="2" t="s">
@@ -7150,7 +7121,7 @@
       <c r="A31" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="19">
         <v>418933</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -7162,10 +7133,10 @@
       <c r="E31" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F31" s="20">
         <v>39.9</v>
       </c>
-      <c r="G31" s="23">
+      <c r="G31" s="20">
         <v>399</v>
       </c>
       <c r="H31" s="2" t="s">
@@ -7194,7 +7165,7 @@
       <c r="A32" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B32" s="22">
+      <c r="B32" s="19">
         <v>446289</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -7206,10 +7177,10 @@
       <c r="E32" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="20">
         <v>322.64</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="20">
         <v>689</v>
       </c>
       <c r="H32" s="2" t="s">
@@ -7238,7 +7209,7 @@
       <c r="A33" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="19">
         <v>457600</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -7250,10 +7221,10 @@
       <c r="E33" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="20">
         <v>384.27</v>
       </c>
-      <c r="G33" s="23">
+      <c r="G33" s="20">
         <v>543</v>
       </c>
       <c r="H33" s="2" t="s">
@@ -7282,7 +7253,7 @@
       <c r="A34" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B34" s="22">
+      <c r="B34" s="19">
         <v>458000</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -7294,10 +7265,10 @@
       <c r="E34" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="20">
         <v>259.57</v>
       </c>
-      <c r="G34" s="23">
+      <c r="G34" s="20">
         <v>625</v>
       </c>
       <c r="H34" s="2" t="s">
@@ -7326,7 +7297,7 @@
       <c r="A35" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B35" s="22">
+      <c r="B35" s="19">
         <v>462680</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -7338,10 +7309,10 @@
       <c r="E35" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="20">
         <v>516</v>
       </c>
-      <c r="G35" s="23">
+      <c r="G35" s="20">
         <v>1200</v>
       </c>
       <c r="H35" s="2" t="s">
@@ -7370,7 +7341,7 @@
       <c r="A36" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B36" s="22">
+      <c r="B36" s="19">
         <v>453275</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -7382,10 +7353,10 @@
       <c r="E36" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="20">
         <v>804.05</v>
       </c>
-      <c r="G36" s="23">
+      <c r="G36" s="20">
         <v>1090</v>
       </c>
       <c r="H36" s="2" t="s">
@@ -7414,7 +7385,7 @@
       <c r="A37" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B37" s="22">
+      <c r="B37" s="19">
         <v>453276</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -7426,10 +7397,10 @@
       <c r="E37" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="20">
         <v>804.05</v>
       </c>
-      <c r="G37" s="23">
+      <c r="G37" s="20">
         <v>1090</v>
       </c>
       <c r="H37" s="2" t="s">
@@ -7458,7 +7429,7 @@
       <c r="A38" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B38" s="22">
+      <c r="B38" s="19">
         <v>453277</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -7470,10 +7441,10 @@
       <c r="E38" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="20">
         <v>804.05</v>
       </c>
-      <c r="G38" s="23">
+      <c r="G38" s="20">
         <v>1090</v>
       </c>
       <c r="H38" s="2" t="s">
@@ -7502,7 +7473,7 @@
       <c r="A39" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B39" s="22">
+      <c r="B39" s="19">
         <v>453278</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -7514,10 +7485,10 @@
       <c r="E39" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="20">
         <v>804.05</v>
       </c>
-      <c r="G39" s="23">
+      <c r="G39" s="20">
         <v>1090</v>
       </c>
       <c r="H39" s="2" t="s">
@@ -7546,7 +7517,7 @@
       <c r="A40" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B40" s="22">
+      <c r="B40" s="19">
         <v>453279</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -7558,10 +7529,10 @@
       <c r="E40" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="20">
         <v>804.05</v>
       </c>
-      <c r="G40" s="23">
+      <c r="G40" s="20">
         <v>1090</v>
       </c>
       <c r="H40" s="2" t="s">
@@ -7590,7 +7561,7 @@
       <c r="A41" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B41" s="22">
+      <c r="B41" s="19">
         <v>460089</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -7602,10 +7573,10 @@
       <c r="E41" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="20">
         <v>7951.05</v>
       </c>
-      <c r="G41" s="23">
+      <c r="G41" s="20">
         <v>15289.93</v>
       </c>
       <c r="H41" s="2" t="s">
@@ -7634,7 +7605,7 @@
       <c r="A42" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B42" s="22">
+      <c r="B42" s="19">
         <v>460378</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -7646,10 +7617,10 @@
       <c r="E42" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="20">
         <v>881.6</v>
       </c>
-      <c r="G42" s="23">
+      <c r="G42" s="20">
         <v>1160</v>
       </c>
       <c r="H42" s="2" t="s">
@@ -7678,7 +7649,7 @@
       <c r="A43" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B43" s="22">
+      <c r="B43" s="19">
         <v>460379</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -7690,10 +7661,10 @@
       <c r="E43" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F43" s="20">
         <v>881.6</v>
       </c>
-      <c r="G43" s="23">
+      <c r="G43" s="20">
         <v>1160</v>
       </c>
       <c r="H43" s="2" t="s">
@@ -7722,7 +7693,7 @@
       <c r="A44" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B44" s="22">
+      <c r="B44" s="19">
         <v>460380</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -7734,10 +7705,10 @@
       <c r="E44" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="F44" s="23">
+      <c r="F44" s="20">
         <v>881.6</v>
       </c>
-      <c r="G44" s="23">
+      <c r="G44" s="20">
         <v>1160</v>
       </c>
       <c r="H44" s="2" t="s">
@@ -7766,7 +7737,7 @@
       <c r="A45" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B45" s="22">
+      <c r="B45" s="19">
         <v>460381</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -7778,10 +7749,10 @@
       <c r="E45" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="F45" s="23">
+      <c r="F45" s="20">
         <v>881.6</v>
       </c>
-      <c r="G45" s="23">
+      <c r="G45" s="20">
         <v>1160</v>
       </c>
       <c r="H45" s="2" t="s">
@@ -7810,7 +7781,7 @@
       <c r="A46" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B46" s="22">
+      <c r="B46" s="19">
         <v>460389</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -7822,10 +7793,10 @@
       <c r="E46" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="F46" s="23">
+      <c r="F46" s="20">
         <v>4131.41</v>
       </c>
-      <c r="G46" s="23">
+      <c r="G46" s="20">
         <v>5436.05</v>
       </c>
       <c r="H46" s="2" t="s">
@@ -7854,7 +7825,7 @@
       <c r="A47" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B47" s="22">
+      <c r="B47" s="19">
         <v>460390</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -7866,10 +7837,10 @@
       <c r="E47" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="F47" s="23">
+      <c r="F47" s="20">
         <v>4131.41</v>
       </c>
-      <c r="G47" s="23">
+      <c r="G47" s="20">
         <v>5436.05</v>
       </c>
       <c r="H47" s="2" t="s">
@@ -7898,7 +7869,7 @@
       <c r="A48" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B48" s="22">
+      <c r="B48" s="19">
         <v>460391</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -7910,10 +7881,10 @@
       <c r="E48" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="F48" s="23">
+      <c r="F48" s="20">
         <v>4131.41</v>
       </c>
-      <c r="G48" s="23">
+      <c r="G48" s="20">
         <v>5436.05</v>
       </c>
       <c r="H48" s="2" t="s">
@@ -7942,7 +7913,7 @@
       <c r="A49" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B49" s="22">
+      <c r="B49" s="19">
         <v>460392</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -7954,10 +7925,10 @@
       <c r="E49" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="F49" s="23">
+      <c r="F49" s="20">
         <v>4131.41</v>
       </c>
-      <c r="G49" s="23">
+      <c r="G49" s="20">
         <v>5436.05</v>
       </c>
       <c r="H49" s="2" t="s">
@@ -7986,7 +7957,7 @@
       <c r="A50" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B50" s="22">
+      <c r="B50" s="19">
         <v>460406</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -7998,10 +7969,10 @@
       <c r="E50" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="F50" s="23">
+      <c r="F50" s="20">
         <v>478.11</v>
       </c>
-      <c r="G50" s="23">
+      <c r="G50" s="20">
         <v>919.39</v>
       </c>
       <c r="H50" s="2" t="s">
@@ -8030,7 +8001,7 @@
       <c r="A51" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B51" s="22">
+      <c r="B51" s="19">
         <v>460407</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -8042,10 +8013,10 @@
       <c r="E51" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="F51" s="23">
+      <c r="F51" s="20">
         <v>478.11</v>
       </c>
-      <c r="G51" s="23">
+      <c r="G51" s="20">
         <v>919.39</v>
       </c>
       <c r="H51" s="2" t="s">
@@ -8074,7 +8045,7 @@
       <c r="A52" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B52" s="22">
+      <c r="B52" s="19">
         <v>460408</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -8086,10 +8057,10 @@
       <c r="E52" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="F52" s="23">
+      <c r="F52" s="20">
         <v>478.11</v>
       </c>
-      <c r="G52" s="23">
+      <c r="G52" s="20">
         <v>919.39</v>
       </c>
       <c r="H52" s="2" t="s">
@@ -8118,7 +8089,7 @@
       <c r="A53" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B53" s="22">
+      <c r="B53" s="19">
         <v>460409</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -8130,10 +8101,10 @@
       <c r="E53" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="F53" s="23">
+      <c r="F53" s="20">
         <v>478.11</v>
       </c>
-      <c r="G53" s="23">
+      <c r="G53" s="20">
         <v>919.39</v>
       </c>
       <c r="H53" s="2" t="s">
@@ -8162,7 +8133,7 @@
       <c r="A54" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B54" s="22">
+      <c r="B54" s="19">
         <v>460410</v>
       </c>
       <c r="C54" s="2" t="s">
@@ -8174,10 +8145,10 @@
       <c r="E54" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="F54" s="23">
+      <c r="F54" s="20">
         <v>478.11</v>
       </c>
-      <c r="G54" s="23">
+      <c r="G54" s="20">
         <v>919.39</v>
       </c>
       <c r="H54" s="2" t="s">
@@ -8206,7 +8177,7 @@
       <c r="A55" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B55" s="22">
+      <c r="B55" s="19">
         <v>460411</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -8218,10 +8189,10 @@
       <c r="E55" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="F55" s="23">
+      <c r="F55" s="20">
         <v>478.11</v>
       </c>
-      <c r="G55" s="23">
+      <c r="G55" s="20">
         <v>919.39</v>
       </c>
       <c r="H55" s="2" t="s">
@@ -8250,7 +8221,7 @@
       <c r="A56" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B56" s="22">
+      <c r="B56" s="19">
         <v>461015</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -8262,10 +8233,10 @@
       <c r="E56" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="F56" s="23">
+      <c r="F56" s="20">
         <v>2885.75</v>
       </c>
-      <c r="G56" s="23">
+      <c r="G56" s="20">
         <v>4850</v>
       </c>
       <c r="H56" s="2" t="s">
@@ -8294,7 +8265,7 @@
       <c r="A57" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B57" s="22">
+      <c r="B57" s="19">
         <v>461016</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -8306,10 +8277,10 @@
       <c r="E57" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="F57" s="23">
+      <c r="F57" s="20">
         <v>577.15</v>
       </c>
-      <c r="G57" s="23">
+      <c r="G57" s="20">
         <v>970</v>
       </c>
       <c r="H57" s="2" t="s">
@@ -8338,7 +8309,7 @@
       <c r="A58" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B58" s="22">
+      <c r="B58" s="19">
         <v>461017</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -8350,10 +8321,10 @@
       <c r="E58" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="F58" s="23">
+      <c r="F58" s="20">
         <v>577.15</v>
       </c>
-      <c r="G58" s="23">
+      <c r="G58" s="20">
         <v>970</v>
       </c>
       <c r="H58" s="2" t="s">
@@ -8382,7 +8353,7 @@
       <c r="A59" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B59" s="22">
+      <c r="B59" s="19">
         <v>461018</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -8394,10 +8365,10 @@
       <c r="E59" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="F59" s="23">
+      <c r="F59" s="20">
         <v>661.33</v>
       </c>
-      <c r="G59" s="23">
+      <c r="G59" s="20">
         <v>829</v>
       </c>
       <c r="H59" s="2" t="s">
@@ -8426,7 +8397,7 @@
       <c r="A60" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B60" s="22">
+      <c r="B60" s="19">
         <v>461019</v>
       </c>
       <c r="C60" s="2" t="s">
@@ -8438,10 +8409,10 @@
       <c r="E60" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="F60" s="23">
+      <c r="F60" s="20">
         <v>661.33</v>
       </c>
-      <c r="G60" s="23">
+      <c r="G60" s="20">
         <v>829</v>
       </c>
       <c r="H60" s="2" t="s">
@@ -8470,7 +8441,7 @@
       <c r="A61" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B61" s="22">
+      <c r="B61" s="19">
         <v>461020</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -8482,10 +8453,10 @@
       <c r="E61" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="F61" s="23">
+      <c r="F61" s="20">
         <v>661.33</v>
       </c>
-      <c r="G61" s="23">
+      <c r="G61" s="20">
         <v>829</v>
       </c>
       <c r="H61" s="2" t="s">
@@ -8514,7 +8485,7 @@
       <c r="A62" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B62" s="22">
+      <c r="B62" s="19">
         <v>461021</v>
       </c>
       <c r="C62" s="2" t="s">
@@ -8526,10 +8497,10 @@
       <c r="E62" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="F62" s="23">
+      <c r="F62" s="20">
         <v>789.66</v>
       </c>
-      <c r="G62" s="23">
+      <c r="G62" s="20">
         <v>990</v>
       </c>
       <c r="H62" s="2" t="s">
@@ -8558,7 +8529,7 @@
       <c r="A63" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B63" s="22">
+      <c r="B63" s="19">
         <v>461022</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -8570,10 +8541,10 @@
       <c r="E63" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="F63" s="23">
+      <c r="F63" s="20">
         <v>789.66</v>
       </c>
-      <c r="G63" s="23">
+      <c r="G63" s="20">
         <v>990</v>
       </c>
       <c r="H63" s="2" t="s">
@@ -8602,7 +8573,7 @@
       <c r="A64" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B64" s="22">
+      <c r="B64" s="19">
         <v>461023</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -8614,10 +8585,10 @@
       <c r="E64" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="F64" s="23">
+      <c r="F64" s="20">
         <v>2490.21</v>
       </c>
-      <c r="G64" s="23">
+      <c r="G64" s="20">
         <v>4185</v>
       </c>
       <c r="H64" s="2" t="s">
@@ -8646,7 +8617,7 @@
       <c r="A65" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B65" s="22">
+      <c r="B65" s="19">
         <v>461024</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -8658,10 +8629,10 @@
       <c r="E65" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="F65" s="23">
+      <c r="F65" s="20">
         <v>2490.21</v>
       </c>
-      <c r="G65" s="23">
+      <c r="G65" s="20">
         <v>4185</v>
       </c>
       <c r="H65" s="2" t="s">
@@ -8690,7 +8661,7 @@
       <c r="A66" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B66" s="22">
+      <c r="B66" s="19">
         <v>461025</v>
       </c>
       <c r="C66" s="2" t="s">
@@ -8702,10 +8673,10 @@
       <c r="E66" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="F66" s="23">
+      <c r="F66" s="20">
         <v>594.54</v>
       </c>
-      <c r="G66" s="23">
+      <c r="G66" s="20">
         <v>999</v>
       </c>
       <c r="H66" s="2" t="s">
@@ -8734,7 +8705,7 @@
       <c r="A67" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B67" s="22">
+      <c r="B67" s="19">
         <v>461026</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -8746,10 +8717,10 @@
       <c r="E67" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="F67" s="23">
+      <c r="F67" s="20">
         <v>594.54</v>
       </c>
-      <c r="G67" s="23">
+      <c r="G67" s="20">
         <v>999</v>
       </c>
       <c r="H67" s="2" t="s">
@@ -8778,7 +8749,7 @@
       <c r="A68" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B68" s="22">
+      <c r="B68" s="19">
         <v>461027</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -8790,10 +8761,10 @@
       <c r="E68" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="F68" s="23">
+      <c r="F68" s="20">
         <v>1251.48</v>
       </c>
-      <c r="G68" s="23">
+      <c r="G68" s="20">
         <v>1569</v>
       </c>
       <c r="H68" s="2" t="s">
@@ -8822,7 +8793,7 @@
       <c r="A69" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B69" s="22">
+      <c r="B69" s="19">
         <v>463074</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -8834,10 +8805,10 @@
       <c r="E69" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="F69" s="23">
+      <c r="F69" s="20">
         <v>772</v>
       </c>
-      <c r="G69" s="23">
+      <c r="G69" s="20">
         <v>950</v>
       </c>
       <c r="H69" s="2" t="s">
@@ -8866,7 +8837,7 @@
       <c r="A70" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B70" s="22">
+      <c r="B70" s="19">
         <v>463075</v>
       </c>
       <c r="C70" s="2" t="s">
@@ -8878,10 +8849,10 @@
       <c r="E70" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="F70" s="23">
+      <c r="F70" s="20">
         <v>772</v>
       </c>
-      <c r="G70" s="23">
+      <c r="G70" s="20">
         <v>950</v>
       </c>
       <c r="H70" s="2" t="s">
@@ -8910,7 +8881,7 @@
       <c r="A71" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B71" s="22">
+      <c r="B71" s="19">
         <v>458997</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -8922,10 +8893,10 @@
       <c r="E71" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="F71" s="23">
+      <c r="F71" s="20">
         <v>2068.08</v>
       </c>
-      <c r="G71" s="23">
+      <c r="G71" s="20">
         <v>2350</v>
       </c>
       <c r="H71" s="2" t="s">
@@ -8954,7 +8925,7 @@
       <c r="A72" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B72" s="22">
+      <c r="B72" s="19">
         <v>458998</v>
       </c>
       <c r="C72" s="2" t="s">
@@ -8966,10 +8937,10 @@
       <c r="E72" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="F72" s="23">
+      <c r="F72" s="20">
         <v>661.2</v>
       </c>
-      <c r="G72" s="23">
+      <c r="G72" s="20">
         <v>870</v>
       </c>
       <c r="H72" s="2" t="s">
@@ -8998,7 +8969,7 @@
       <c r="A73" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B73" s="22">
+      <c r="B73" s="19">
         <v>581314</v>
       </c>
       <c r="C73" s="2" t="s">
@@ -9010,10 +8981,10 @@
       <c r="E73" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="F73" s="23">
+      <c r="F73" s="20">
         <v>4257.83</v>
       </c>
-      <c r="G73" s="23">
+      <c r="G73" s="20">
         <v>4290</v>
       </c>
       <c r="H73" s="2" t="s">
@@ -9042,7 +9013,7 @@
       <c r="A74" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B74" s="22">
+      <c r="B74" s="19">
         <v>581315</v>
       </c>
       <c r="C74" s="2" t="s">
@@ -9054,10 +9025,10 @@
       <c r="E74" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="F74" s="23">
+      <c r="F74" s="20">
         <v>4257.83</v>
       </c>
-      <c r="G74" s="23">
+      <c r="G74" s="20">
         <v>4290</v>
       </c>
       <c r="H74" s="2" t="s">
@@ -9086,7 +9057,7 @@
       <c r="A75" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B75" s="22">
+      <c r="B75" s="19">
         <v>581316</v>
       </c>
       <c r="C75" s="2" t="s">
@@ -9098,10 +9069,10 @@
       <c r="E75" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="F75" s="23">
+      <c r="F75" s="20">
         <v>1207.8800000000001</v>
       </c>
-      <c r="G75" s="23">
+      <c r="G75" s="20">
         <v>1217</v>
       </c>
       <c r="H75" s="2" t="s">
@@ -9130,7 +9101,7 @@
       <c r="A76" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B76" s="22">
+      <c r="B76" s="19">
         <v>581317</v>
       </c>
       <c r="C76" s="2" t="s">
@@ -9142,10 +9113,10 @@
       <c r="E76" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="F76" s="23">
+      <c r="F76" s="20">
         <v>4317.38</v>
       </c>
-      <c r="G76" s="23">
+      <c r="G76" s="20">
         <v>4350</v>
       </c>
       <c r="H76" s="2" t="s">
@@ -9174,7 +9145,7 @@
       <c r="A77" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B77" s="22">
+      <c r="B77" s="19">
         <v>581318</v>
       </c>
       <c r="C77" s="2" t="s">
@@ -9186,10 +9157,10 @@
       <c r="E77" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="F77" s="23">
+      <c r="F77" s="20">
         <v>3437.65</v>
       </c>
-      <c r="G77" s="23">
+      <c r="G77" s="20">
         <v>3490</v>
       </c>
       <c r="H77" s="2" t="s">
@@ -9228,14 +9199,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>380</v>
       </c>
     </row>
@@ -9266,46 +9237,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>381</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>384</v>
       </c>
     </row>
@@ -9330,54 +9301,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>387</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>389</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>393</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>395</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>396</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>400</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>401</v>
       </c>
     </row>
@@ -9388,19 +9360,19 @@
       <c r="B2" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45717</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="28">
         <v>2330</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="28" t="s">
         <v>403</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="29">
         <v>7431</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="29">
         <v>1129</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -9418,13 +9390,13 @@
       <c r="L2" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="30" t="s">
         <v>405</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="31" t="s">
         <v>406</v>
       </c>
     </row>
@@ -9455,26 +9427,25 @@
       <c r="B1" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="32" t="s">
         <v>408</v>
       </c>
-      <c r="E1" s="36">
-        <f>SUM(B2:B157)</f>
-        <v>104</v>
-      </c>
-      <c r="F1" s="37">
+      <c r="E1" s="33">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="36">
         <f>53+51</f>
         <v>104</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="34">
         <v>6.877397169686549E-3</v>
       </c>
     </row>

</xml_diff>